<commit_message>
MooveSpeed -> MovementSpeed 이름 수정
</commit_message>
<xml_diff>
--- a/XLSX/MonsterTable.xlsx
+++ b/XLSX/MonsterTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CProject\SProject\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF8E7DF-0FC8-4B2D-9F1B-1BC82BC25828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267038A8-1A14-4008-8088-285395597AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
   </bookViews>
   <sheets>
     <sheet name="!Monster" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>AttackSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,13 +205,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MooveSpeed</t>
-  </si>
-  <si>
-    <t>MooveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>float32</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -252,6 +245,10 @@
   </si>
   <si>
     <t>Class&lt;AStageMonsterUnit&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MovementSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -686,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3F3863-F070-4592-A50F-8035B6750A51}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -701,7 +698,7 @@
     <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="7.75" customWidth="1"/>
     <col min="12" max="12" width="14.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.375" bestFit="1" customWidth="1"/>
@@ -713,7 +710,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -731,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -740,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>7</v>
@@ -761,10 +758,10 @@
         <v>41</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -778,10 +775,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>36</v>
@@ -793,13 +790,13 @@
         <v>36</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>36</v>
@@ -808,7 +805,7 @@
         <v>36</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>36</v>
@@ -817,10 +814,10 @@
         <v>36</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -834,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -886,13 +883,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40697F6B-D6AA-4A3C-BC30-5A6A92BE5A91}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" customWidth="1"/>
     <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -906,7 +903,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
@@ -1011,75 +1008,75 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
+      <c r="A10" t="s">
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>